<commit_message>
Added Ability to get Required Column Ids from column name colour
</commit_message>
<xml_diff>
--- a/Project/src/test/java/com/model/utilities/testFile1.xlsx
+++ b/Project/src/test/java/com/model/utilities/testFile1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leo/Documents/GitHub/Team11/Project/src/com/test/model/utilities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leo/Documents/GitHub/Team11/Project/src/test/java/com/model/utilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6C88BB-CCAB-8F47-B104-1E603C408ADF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA716FC-CD7F-E644-9E2B-6A47D88BBA44}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16080" activeTab="1" xr2:uid="{447609F5-85B7-7142-9598-C5D49E352059}"/>
   </bookViews>
@@ -104,7 +104,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -135,6 +135,13 @@
     <font>
       <sz val="18"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFA500"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -187,9 +194,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -511,18 +519,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92293B13-9F26-F043-AD04-113AE6EC81AC}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:C5"/>
+    <sheetView zoomScale="215" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="123" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -536,10 +544,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -580,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95FCDAAA-6521-904F-9272-DEBE0CF02169}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -592,11 +600,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="121" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -610,7 +618,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">

</xml_diff>